<commit_message>
Fixed power total to Node Enclosure since fan is now not going through node enclosure
</commit_message>
<xml_diff>
--- a/Node Power and cooling.xlsx
+++ b/Node Power and cooling.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18067"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MRD\EoR\HERA\Node\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zara\Documents\node-doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="82">
   <si>
     <t>White Rabbit</t>
   </si>
@@ -248,9 +248,6 @@
     <t>Inrush Input VAC currents</t>
   </si>
   <si>
-    <t>includes current for FEM and external centrifugal fan</t>
-  </si>
-  <si>
     <t>total guess for the TBD Lineare power supply inrush</t>
   </si>
   <si>
@@ -267,12 +264,18 @@
   </si>
   <si>
     <t>This heat will be handled by long run of buried ducting between the centrifugal fan and the Node Enclosure</t>
+  </si>
+  <si>
+    <t>VAC current input to the Node (Total)</t>
+  </si>
+  <si>
+    <t>Includes current for FEM and external centrifugal fan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -696,19 +699,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="60" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.15625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.15625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="54" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="18.3" x14ac:dyDescent="0.7">
       <c r="B3" s="9" t="s">
         <v>47</v>
       </c>
@@ -716,7 +719,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="9" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
       <c r="A4" s="11" t="s">
         <v>4</v>
       </c>
@@ -737,7 +740,7 @@
       </c>
       <c r="G4" s="13"/>
     </row>
-    <row r="5" spans="1:7" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="9" customFormat="1" ht="18.3" x14ac:dyDescent="0.7">
       <c r="B5" s="10" t="s">
         <v>62</v>
       </c>
@@ -754,7 +757,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -780,7 +783,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -803,7 +806,7 @@
         <v>28.349999999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -825,7 +828,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -847,7 +850,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>60</v>
       </c>
@@ -872,7 +875,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -894,7 +897,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -916,7 +919,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
         <v>50</v>
       </c>
@@ -938,7 +941,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
         <v>51</v>
       </c>
@@ -960,7 +963,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -982,7 +985,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>63</v>
       </c>
@@ -1006,7 +1009,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1015,7 +1018,7 @@
         <v>302.5</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:7" s="14" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A20" s="14" t="s">
         <v>65</v>
       </c>
@@ -1025,9 +1028,9 @@
       </c>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:7" s="14" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A21" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F21" s="14">
         <f>F6</f>
@@ -1035,22 +1038,22 @@
       </c>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" s="14" customFormat="1" ht="31.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.75">
       <c r="A22" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F22" s="14">
         <f>F16</f>
         <v>66</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="14" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="14" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="G23" s="12"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>66</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>72</v>
       </c>
@@ -1069,7 +1072,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>53</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1099,7 +1102,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="1" t="s">
         <v>50</v>
       </c>
@@ -1111,7 +1114,7 @@
         <v>0.56100981767180924</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
         <v>51</v>
       </c>
@@ -1123,7 +1126,7 @@
         <v>0.12856474988312294</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>63</v>
       </c>
@@ -1139,34 +1142,43 @@
         <v>71</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
       <c r="A34" s="14" t="s">
         <v>70</v>
       </c>
       <c r="C34" s="18">
-        <f>SUM(C28:C33)</f>
-        <v>1.6048922933074408</v>
-      </c>
-      <c r="G34" s="12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+        <f>SUM(C29:C31)</f>
+        <v>1.1109792498291795</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
+      <c r="A35" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="C35" s="18">
+        <f>SUM(C32,C34,C28)</f>
+        <v>1.6048922933074405</v>
+      </c>
+      <c r="G35" s="12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
         <v>53</v>
       </c>
@@ -1174,10 +1186,10 @@
         <v>40</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
         <v>57</v>
       </c>
@@ -1185,10 +1197,10 @@
         <v>40</v>
       </c>
       <c r="G41" s="12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="1" t="s">
         <v>50</v>
       </c>
@@ -1196,7 +1208,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="1" t="s">
         <v>51</v>
       </c>
@@ -1204,12 +1216,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
         <v>5</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
         <v>5</v>
       </c>
@@ -1232,7 +1244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
         <v>7</v>
       </c>
@@ -1243,7 +1255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
         <v>15</v>
       </c>
@@ -1254,7 +1266,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
         <v>16</v>
       </c>
@@ -1266,7 +1278,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
         <v>17</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
         <v>11</v>
       </c>
@@ -1290,7 +1302,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B56">
         <f>B55/60</f>
         <v>5.8890188293456509</v>
@@ -1299,7 +1311,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="B57">
         <f>B56/0.33048</f>
         <v>17.819592197245374</v>
@@ -1308,12 +1320,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="6" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
         <v>19</v>
       </c>
@@ -1324,7 +1336,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
         <v>23</v>
       </c>
@@ -1339,7 +1351,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B65">
         <f>(B64/POWER(12,2))*POWER(0.3048,2)</f>
         <v>5.1612800000000007E-2</v>
@@ -1348,7 +1360,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
         <v>25</v>
       </c>
@@ -1359,7 +1371,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
         <v>27</v>
       </c>
@@ -1370,7 +1382,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
         <v>29</v>
       </c>
@@ -1381,7 +1393,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
         <v>30</v>
       </c>
@@ -1392,7 +1404,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
         <v>31</v>
       </c>
@@ -1403,7 +1415,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
         <v>32</v>
       </c>
@@ -1414,7 +1426,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
         <v>33</v>
       </c>
@@ -1426,7 +1438,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
         <v>40</v>
       </c>
@@ -1434,7 +1446,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
         <v>34</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -1458,7 +1470,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" t="s">
         <v>35</v>
       </c>
@@ -1469,7 +1481,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" t="s">
         <v>36</v>
       </c>
@@ -1480,7 +1492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" t="s">
         <v>37</v>
       </c>
@@ -1491,7 +1503,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
Included FEM to Node Enclosure
</commit_message>
<xml_diff>
--- a/Node Power and cooling.xlsx
+++ b/Node Power and cooling.xlsx
@@ -269,7 +269,7 @@
     <t>VAC current input to the Node (Total)</t>
   </si>
   <si>
-    <t>Includes current for FEM and external centrifugal fan</t>
+    <t>Includes current for external centrifugal fan</t>
   </si>
 </sst>
 </file>
@@ -699,8 +699,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:G83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1147,8 +1147,8 @@
         <v>70</v>
       </c>
       <c r="C34" s="18">
-        <f>SUM(C29:C31)</f>
-        <v>1.1109792498291795</v>
+        <f>SUM(C28:C31)</f>
+        <v>1.2848922933074407</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="20.399999999999999" x14ac:dyDescent="0.75">
@@ -1156,8 +1156,8 @@
         <v>80</v>
       </c>
       <c r="C35" s="18">
-        <f>SUM(C32,C34,C28)</f>
-        <v>1.6048922933074405</v>
+        <f>SUM(C32,C34)</f>
+        <v>1.6048922933074408</v>
       </c>
       <c r="G35" s="12" t="s">
         <v>81</v>

</xml_diff>